<commit_message>
basic methods tested, consumer demand assignment corrected
</commit_message>
<xml_diff>
--- a/test_agents_sheets/test.xlsx
+++ b/test_agents_sheets/test.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>5.5</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>r</t>
   </si>
@@ -396,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K3" sqref="K3:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -420,51 +417,51 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1">
         <v>0.99</v>
@@ -490,13 +487,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
@@ -525,16 +522,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>220</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>150</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5.5</v>
       </c>
       <c r="E4" s="1">
         <v>0.99</v>
@@ -653,10 +650,6 @@
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="2"/>
-      <c r="D29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>